<commit_message>
version tres de testeo lista de chequeo
</commit_message>
<xml_diff>
--- a/Lista de chequeo.xlsx
+++ b/Lista de chequeo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E1E695-3C22-4DBD-BAF0-FC1CB9CEAF43}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D0AB391-02B0-4005-8D28-CC83BA9503B6}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     <t>ID 07</t>
   </si>
   <si>
-    <t>¿Como cajero tiene un buena organizacion en su espacio?</t>
+    <t>¿Está usted satisfecho con los tiempos de espera?</t>
   </si>
   <si>
     <t>ID 08</t>
@@ -825,205 +825,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:I18"/>
+  <dimension ref="C4:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" ht="39.75" customHeight="1">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="3:8" ht="33.75">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="4:9" ht="31.5" customHeight="1">
-      <c r="D5" s="5" t="s">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="3:8" ht="31.5" customHeight="1">
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="4:9">
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="3:8">
+      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="4:9">
-      <c r="D7" s="15" t="s">
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="3:8">
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="G7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="H7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="4:9" ht="38.25" customHeight="1">
-      <c r="D8" s="15" t="s">
+    <row r="8" spans="3:8" ht="44.25" customHeight="1">
+      <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="D8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="4:9" ht="30" customHeight="1">
-      <c r="D9" s="15" t="s">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="3:8" ht="34.5" customHeight="1">
+      <c r="C9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="4:9" ht="42.75" customHeight="1">
-      <c r="D10" s="15" t="s">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="3:8" ht="46.5" customHeight="1">
+      <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="23" t="s">
         <v>15</v>
       </c>
+      <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="4:9" ht="42" customHeight="1">
-      <c r="D11" s="15" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="3:8" ht="45" customHeight="1">
+      <c r="C11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="D11" s="23" t="s">
         <v>17</v>
       </c>
+      <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="4:9" ht="33.75" customHeight="1">
-      <c r="D12" s="15" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="3:8" ht="44.25" customHeight="1">
+      <c r="C12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="D12" s="23" t="s">
         <v>19</v>
       </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="4:9" ht="40.5" customHeight="1">
-      <c r="D13" s="25" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="3:8" ht="48.75" customHeight="1">
+      <c r="C13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="26" t="s">
         <v>21</v>
       </c>
+      <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="4:9" ht="33.75" customHeight="1">
-      <c r="D14" s="27" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="3:8" ht="48" customHeight="1">
+      <c r="C14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="4:9" ht="46.5" customHeight="1">
-      <c r="D15" s="27" t="s">
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="3:8" ht="73.5" customHeight="1">
+      <c r="C15" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="23" t="s">
         <v>25</v>
       </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="4:9" ht="35.25" customHeight="1">
-      <c r="D16" s="27" t="s">
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="3:8" ht="73.5" customHeight="1">
+      <c r="C16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="23" t="s">
         <v>27</v>
       </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="4:9" ht="43.5" customHeight="1">
-      <c r="D17" s="27" t="s">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="3:8" ht="63" customHeight="1">
+      <c r="C17" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="D17" s="23" t="s">
         <v>29</v>
       </c>
+      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="4:9" ht="54.75" customHeight="1">
-      <c r="D18" s="28" t="s">
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="3:8" ht="63.75" customHeight="1">
+      <c r="C18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="D18" s="29" t="s">
         <v>31</v>
       </c>
+      <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
+      <c r="H18" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lista de chequeo version dos
</commit_message>
<xml_diff>
--- a/Lista de chequeo.xlsx
+++ b/Lista de chequeo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D0AB391-02B0-4005-8D28-CC83BA9503B6}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E1E695-3C22-4DBD-BAF0-FC1CB9CEAF43}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     <t>ID 07</t>
   </si>
   <si>
-    <t>¿Está usted satisfecho con los tiempos de espera?</t>
+    <t>¿Como cajero tiene un buena organizacion en su espacio?</t>
   </si>
   <si>
     <t>ID 08</t>
@@ -825,205 +825,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:H18"/>
+  <dimension ref="D4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="35" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" ht="33.75">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="4:9" ht="39.75" customHeight="1">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="3:8" ht="31.5" customHeight="1">
-      <c r="C5" s="5" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="4:9" ht="31.5" customHeight="1">
+      <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="3:8">
-      <c r="C6" s="10"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="4:9">
       <c r="D6" s="10"/>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="3:8">
-      <c r="C7" s="15" t="s">
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="4:9">
+      <c r="D7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="44.25" customHeight="1">
-      <c r="C8" s="15" t="s">
+    <row r="8" spans="4:9" ht="38.25" customHeight="1">
+      <c r="D8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="E8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="14"/>
-    </row>
-    <row r="9" spans="3:8" ht="34.5" customHeight="1">
-      <c r="C9" s="15" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="4:9" ht="30" customHeight="1">
+      <c r="D9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="3:8" ht="46.5" customHeight="1">
-      <c r="C10" s="15" t="s">
+      <c r="H9" s="21"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="4:9" ht="42.75" customHeight="1">
+      <c r="D10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="3:8" ht="45" customHeight="1">
-      <c r="C11" s="15" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="4:9" ht="42" customHeight="1">
+      <c r="D11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="E11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="3:8" ht="44.25" customHeight="1">
-      <c r="C12" s="15" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="4:9" ht="33.75" customHeight="1">
+      <c r="D12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="E12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="3:8" ht="48.75" customHeight="1">
-      <c r="C13" s="25" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="4:9" ht="40.5" customHeight="1">
+      <c r="D13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="E13" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="3:8" ht="48" customHeight="1">
-      <c r="C14" s="27" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="4:9" ht="33.75" customHeight="1">
+      <c r="D14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="3:8" ht="73.5" customHeight="1">
-      <c r="C15" s="27" t="s">
+      <c r="H14" s="10"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="4:9" ht="46.5" customHeight="1">
+      <c r="D15" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="E15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="3:8" ht="73.5" customHeight="1">
-      <c r="C16" s="27" t="s">
+      <c r="H15" s="10"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="4:9" ht="35.25" customHeight="1">
+      <c r="D16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="E16" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="3:8" ht="63" customHeight="1">
-      <c r="C17" s="27" t="s">
+      <c r="H16" s="10"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="4:9" ht="43.5" customHeight="1">
+      <c r="D17" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="E17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="3:8" ht="63.75" customHeight="1">
-      <c r="C18" s="28" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="4:9" ht="54.75" customHeight="1">
+      <c r="D18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>